<commit_message>
Fix for assessment type and name/link not getting populated in learner submission - typo extra 's' in 'assessment'. Also removed 'ela_' from form field names for consistency. Updated all template files - xml and xlsx.
</commit_message>
<xml_diff>
--- a/ela/templates/ELA_FORM_TMPL_A1.xlsx
+++ b/ela/templates/ELA_FORM_TMPL_A1.xlsx
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="115">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -275,7 +275,7 @@
     <t xml:space="preserve">calculate</t>
   </si>
   <si>
-    <t xml:space="preserve">ela_form_id</t>
+    <t xml:space="preserve">form_id</t>
   </si>
   <si>
     <t xml:space="preserve">“{{ id }}”</t>
@@ -306,7 +306,7 @@
   </si>
   <si>
     <t xml:space="preserve">The following {{ assessment_count }} assessment(s) are included in this form
-{{ question_types[0] }}: {{ ela_asssessment_ids[0]  }}</t>
+{{ question_types[0] }}: {{ assessment_ids[0]  }}</t>
   </si>
   <si>
     <t xml:space="preserve">num_assessments</t>
@@ -369,10 +369,10 @@
     <t xml:space="preserve">{{ question_prompts[0] }}</t>
   </si>
   <si>
-    <t xml:space="preserve">ela_asssessment_id_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“{{ ela_asssessment_ids[0] }}”</t>
+    <t xml:space="preserve">assessment_id_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“{{ assessment_ids[0] }}”</t>
   </si>
   <si>
     <t xml:space="preserve">question_1_type</t>
@@ -526,9 +526,6 @@
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">form_id</t>
   </si>
   <si>
     <t xml:space="preserve">version</t>
@@ -704,10 +701,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="3" sqref="B18 C8 L18 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
@@ -1059,10 +1056,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="A23" activeCellId="3" sqref="B18 C8 L18 A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.63"/>
@@ -1395,10 +1392,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="3" sqref="B18 C8 L18 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.13"/>
@@ -1410,13 +1407,13 @@
         <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1443,10 +1440,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>1</v>
@@ -1472,34 +1469,34 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="3" sqref="B18 C8 L18 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.921875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>